<commit_message>
prototype scene major update
</commit_message>
<xml_diff>
--- a/Documentation/Dark Fantasy Armoury 3D Scene.xlsx
+++ b/Documentation/Dark Fantasy Armoury 3D Scene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni Stuff Portable\Year 3 Uni Work\Module 4\GitHubRepo\Dark-Fantasy-Armoury\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645AC038-79C8-4F2D-866B-A20ABEFDABB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B0811-6F04-467E-8615-86DC6697E48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B5015552-CDE9-4DE5-9684-7753E9E55018}"/>
   </bookViews>
@@ -668,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704DEA17-3E42-4DC1-B731-7742A95B18C6}">
   <dimension ref="B2:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
@@ -1438,20 +1438,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2a85df21-10b5-4e5c-b3bf-86639cf7232c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2a85df21-10b5-4e5c-b3bf-86639cf7232c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,6 +1474,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11E65AE-CCFB-4ECA-9415-F67D2A7AEC27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9E08866-CBB7-4DEA-BEED-0B67211157B1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1488,12 +1496,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11E65AE-CCFB-4ECA-9415-F67D2A7AEC27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>